<commit_message>
syncing the HPE version
</commit_message>
<xml_diff>
--- a/styles/HPE/progress_list.xlsx
+++ b/styles/HPE/progress_list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtceurope-my.sharepoint.com/personal/eric_szegedi_dtc-e_com/Documents/personal_documents/git/vale_linter/styles/HPE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="13_ncr:1_{C8437D09-466C-469D-8559-3163E2B45CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9972F6D3-97FF-46ED-9993-CF3E481B26F8}"/>
+  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{C8437D09-466C-469D-8559-3163E2B45CFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F973A4E5-D05B-483E-8354-6191A8F0DA3E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{EC14D7F9-078E-4114-B177-94F6D1D807CC}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="774" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="385">
   <si>
     <t>Zero</t>
   </si>
@@ -1573,8 +1573,8 @@
   <dimension ref="A1:C389"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J29" sqref="J29"/>
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D141" sqref="D141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1946,9 +1946,6 @@
       <c r="A46" t="s">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
-        <v>374</v>
-      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
@@ -4685,17 +4682,17 @@
       </c>
       <c r="B388">
         <f>COUNTA(B2:B387)</f>
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C388">
         <f>A388-B388</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B389" s="3">
         <f>B388/A388</f>
-        <v>1</v>
+        <v>0.99740932642487046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>